<commit_message>
add type in inserting new event data
</commit_message>
<xml_diff>
--- a/reports/report_2023-09-29.xlsx
+++ b/reports/report_2023-09-29.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,24 +415,30 @@
       <c r="D1" t="str">
         <v>director</v>
       </c>
+      <c r="E1" t="str">
+        <v>writer</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>https://www.imdb.com/title/tt13622776/?ref_=hm_top_tt_i_1</v>
+        <v>https://www.imdb.com/title/tt15426714/?ref_=hm_tpks_tt_i_2_pd_tp1_pbr_ic</v>
       </c>
       <c r="B2" t="str">
-        <v>Ahsoka</v>
+        <v>Wilderness</v>
       </c>
       <c r="C2" t="str">
-        <v>2023–</v>
+        <v>2023</v>
       </c>
       <c r="D2" t="str">
-        <v>Dave Filoni</v>
+        <v>Marnie Dickens</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Jenna Coleman</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>